<commit_message>
fixed excel to pdf function
</commit_message>
<xml_diff>
--- a/StoreManagement/ExcelSheets/boxStamp.xlsx
+++ b/StoreManagement/ExcelSheets/boxStamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\StoreManagement\StoreManagement\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D963E71-05B4-4E24-8D10-AA2B62474AB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{381550AB-8C7E-413F-8F61-A30A4AE41D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -233,7 +233,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BD76DD8-5006-44FE-8E01-53A2EE9E83B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{974BE6B1-6001-4D2E-A45D-C64C8F1C078B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>